<commit_message>
Remove `pax` from databases
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/cea/databases/CH/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10115"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/Documents/GitHub/CityEnergyAnalyst/cea/databases/CH/archetypes/use_types/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4357B94E-AF27-2A41-B00E-E52E64495DEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2930" windowWidth="19340" windowHeight="16460" tabRatio="785"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19540" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERNAL_LOADS" sheetId="7" r:id="rId1"/>
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -120,24 +121,6 @@
     <t>Qcpro_Wm2</t>
   </si>
   <si>
-    <t>Occ_m2pax</t>
-  </si>
-  <si>
-    <t>Vww_lpdpax</t>
-  </si>
-  <si>
-    <t>Vw_lpdpax</t>
-  </si>
-  <si>
-    <t>X_ghpax</t>
-  </si>
-  <si>
-    <t>Qs_Wpax</t>
-  </si>
-  <si>
-    <t>Ve_lpspax</t>
-  </si>
-  <si>
     <t>RH_min_pc</t>
   </si>
   <si>
@@ -148,12 +131,30 @@
   </si>
   <si>
     <t>Ev_kWveh</t>
+  </si>
+  <si>
+    <t>Vww_ldp</t>
+  </si>
+  <si>
+    <t>Vw_ldp</t>
+  </si>
+  <si>
+    <t>X_ghp</t>
+  </si>
+  <si>
+    <t>Qs_Wp</t>
+  </si>
+  <si>
+    <t>Occ_m2p</t>
+  </si>
+  <si>
+    <t>Ve_lsp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -1107,42 +1108,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7265625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7265625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="C1" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>1</v>
@@ -1157,10 +1158,10 @@
         <v>20</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>27</v>
@@ -1172,10 +1173,10 @@
         <v>29</v>
       </c>
       <c r="N1" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1307,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1396,7 +1397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1441,7 +1442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1529,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1710,7 +1711,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1754,7 +1755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -1798,7 +1799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -1889,7 +1890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -1977,7 +1978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -2028,29 +2029,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
@@ -2065,16 +2066,16 @@
         <v>22</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -2155,7 +2156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -2236,7 +2237,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -2290,7 +2291,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -2317,7 +2318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -2371,7 +2372,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -2398,7 +2399,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>17</v>
       </c>
@@ -2450,7 +2451,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>18</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -2503,7 +2504,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
@@ -2530,7 +2531,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>28</v>
       </c>
@@ -2594,9 +2595,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2770,26 +2774,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2813,9 +2806,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add SEMICONDUCTOR and PHARMACEUTICAL use type, and modify databses to store the previously hardcoded parameters
</commit_message>
<xml_diff>
--- a/cea/databases/CH/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
+++ b/cea/databases/CH/archetypes/use_types/USE_TYPE_PROPERTIES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.santos\Documents\CityEnergyAnalyst\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\YTSA01\CS\CityEnergyAnalyst\cea\databases\CH\archetypes\use_types\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EBE8DF2-679A-44B2-BA1F-8BC286C3E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55C8369-99B8-4EA5-B58C-1B744B150192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="785" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDOOR_COMFORT" sheetId="6" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="47">
   <si>
     <t>Ths_set_C</t>
   </si>
@@ -159,14 +159,36 @@
   </si>
   <si>
     <t>Ve_lsp</t>
+  </si>
+  <si>
+    <t>SEMICONDUCTOR</t>
+  </si>
+  <si>
+    <t>PHARMACEUTICAL</t>
+  </si>
+  <si>
+    <t>TCData_Sup</t>
+  </si>
+  <si>
+    <t>TCData_Re</t>
+  </si>
+  <si>
+    <t>Hp_X_Cool</t>
+  </si>
+  <si>
+    <t>Hp_Ratio</t>
+  </si>
+  <si>
+    <t>N_Hs</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -685,7 +707,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -708,12 +730,18 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -770,10 +798,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1039,26 +1063,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.81640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="6" max="6" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -1084,7 +1108,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1111,7 +1135,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1138,7 +1162,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1165,7 +1189,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1192,7 +1216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1219,7 +1243,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
@@ -1246,7 +1270,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
@@ -1273,7 +1297,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
@@ -1300,7 +1324,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
@@ -1327,7 +1351,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
@@ -1354,7 +1378,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1381,7 +1405,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1408,7 +1432,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
@@ -1434,12 +1458,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="4">
         <v>18</v>
@@ -1451,50 +1475,50 @@
         <v>12</v>
       </c>
       <c r="F15" s="7">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G15" s="7">
         <v>30</v>
       </c>
       <c r="H15" s="7">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2">
+        <v>26</v>
+      </c>
+      <c r="C16" s="4">
         <v>18</v>
       </c>
-      <c r="B16" s="2">
-        <v>2</v>
-      </c>
-      <c r="C16" s="4">
-        <v>2</v>
-      </c>
       <c r="D16" s="2">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="E16" s="4">
-        <v>-18</v>
+        <v>12</v>
       </c>
       <c r="F16" s="7">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G16" s="7">
         <v>30</v>
       </c>
       <c r="H16" s="7">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C17" s="4">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2">
         <v>28</v>
@@ -1503,94 +1527,146 @@
         <v>12</v>
       </c>
       <c r="F17" s="7">
+        <v>0</v>
+      </c>
+      <c r="G17" s="7">
+        <v>30</v>
+      </c>
+      <c r="H17" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2">
+        <v>2</v>
+      </c>
+      <c r="C18" s="4">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-18</v>
+      </c>
+      <c r="F18" s="7">
+        <v>0</v>
+      </c>
+      <c r="G18" s="7">
+        <v>30</v>
+      </c>
+      <c r="H18" s="7">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="2">
+        <v>26</v>
+      </c>
+      <c r="C19" s="4">
+        <v>21</v>
+      </c>
+      <c r="D19" s="2">
+        <v>28</v>
+      </c>
+      <c r="E19" s="4">
+        <v>12</v>
+      </c>
+      <c r="F19" s="7">
         <f>20*15/3.6</f>
         <v>83.333333333333329</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G19" s="7">
         <v>30</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H19" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B20" s="2">
         <v>26</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C20" s="4">
         <v>21</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D20" s="2">
         <v>28</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E20" s="4">
         <v>12</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F20" s="7">
         <f>36/3.6</f>
         <v>10</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G20" s="7">
         <v>30</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H20" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B21" s="2">
         <v>26</v>
       </c>
-      <c r="C19" s="4">
+      <c r="C21" s="4">
         <v>21</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D21" s="2">
         <v>28</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E21" s="4">
         <v>12</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F21" s="7">
         <f>36/3.6</f>
         <v>10</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G21" s="7">
         <v>40</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H21" s="7">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B22" s="2">
         <v>26</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C22" s="4">
         <v>21</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D22" s="2">
         <v>28</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E22" s="4">
         <v>12</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F22" s="7">
         <f>30/3.6</f>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G22" s="7">
         <v>30</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H22" s="7">
         <v>60</v>
       </c>
     </row>
@@ -1598,37 +1674,43 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="F2:F20" unlockedFormula="1"/>
+    <ignoredError sqref="F16:F22 F2:F13" unlockedFormula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.453125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="10.453125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6328125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12" style="1" customWidth="1"/>
     <col min="6" max="6" width="10" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.6328125" style="1" customWidth="1"/>
-    <col min="12" max="13" width="12.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="11.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="1" customWidth="1"/>
+    <col min="12" max="13" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="1"/>
+    <col min="15" max="15" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>32</v>
       </c>
@@ -1671,24 +1753,39 @@
       <c r="N1" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <v>30</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="8">
         <v>70</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>80</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="8">
         <v>8</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>2.7</v>
       </c>
       <c r="G2" s="7">
@@ -1697,10 +1794,10 @@
       <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="8">
         <v>35</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <v>140</v>
       </c>
       <c r="K2" s="7">
@@ -1715,12 +1812,27 @@
       <c r="N2" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O2" s="8">
+        <v>7</v>
+      </c>
+      <c r="P2" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R2" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S2" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>50</v>
       </c>
       <c r="C3" s="7">
@@ -1735,16 +1847,16 @@
       <c r="F3" s="7">
         <v>2.7</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>0</v>
       </c>
       <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="8">
         <v>40</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <v>160</v>
       </c>
       <c r="K3" s="7">
@@ -1759,36 +1871,51 @@
       <c r="N3" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O3" s="8">
+        <v>7</v>
+      </c>
+      <c r="P3" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R3" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S3" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>15</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="8">
         <v>70</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>80</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="8">
         <v>8</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="8">
         <v>2.7</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="8">
         <v>0</v>
       </c>
       <c r="H4" s="7">
         <v>0</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="8">
         <v>40</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <v>160</v>
       </c>
       <c r="K4" s="7">
@@ -1803,36 +1930,51 @@
       <c r="N4" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O4" s="8">
+        <v>7</v>
+      </c>
+      <c r="P4" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R4" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S4" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>14</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <v>70</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>80</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="8">
         <v>7</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="8">
         <v>15.9</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="8">
         <v>0</v>
       </c>
       <c r="H5" s="7">
         <v>0</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="8">
         <v>3</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <v>60</v>
       </c>
       <c r="K5" s="7">
@@ -1847,37 +1989,52 @@
       <c r="N5" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O5" s="8">
+        <v>7</v>
+      </c>
+      <c r="P5" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R5" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S5" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>8</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="8">
         <v>70</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="8">
         <v>80</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="8">
         <v>2</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="8">
         <f>9.3+24</f>
         <v>33.299999999999997</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="8">
         <v>0</v>
       </c>
       <c r="H6" s="7">
         <v>0</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="8">
         <v>2</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <v>30</v>
       </c>
       <c r="K6" s="7">
@@ -1892,37 +2049,52 @@
       <c r="N6" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O6" s="8">
+        <v>7</v>
+      </c>
+      <c r="P6" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q6" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S6" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>8</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <v>70</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="8">
         <v>80</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="8">
         <f>9.3+12</f>
         <v>21.3</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="8">
         <v>0</v>
       </c>
       <c r="H7" s="7">
         <v>0</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="8">
         <v>2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <v>30</v>
       </c>
       <c r="K7" s="7">
@@ -1937,36 +2109,51 @@
       <c r="N7" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O7" s="8">
+        <v>7</v>
+      </c>
+      <c r="P7" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q7" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S7" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>2</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="8">
         <v>70</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="8">
         <v>80</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="8">
         <v>6.9</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="8">
         <v>0</v>
       </c>
       <c r="H8" s="7">
         <v>0</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="8">
         <v>15</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <v>45</v>
       </c>
       <c r="K8" s="7">
@@ -1981,36 +2168,51 @@
       <c r="N8" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O8" s="8">
+        <v>7</v>
+      </c>
+      <c r="P8" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R8" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S8" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <v>90</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>170</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>10</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="8">
         <v>10.8</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="8">
         <v>16.5</v>
       </c>
       <c r="H9" s="7">
         <v>0</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="8">
         <v>3</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <v>60</v>
       </c>
       <c r="K9" s="7">
@@ -2025,36 +2227,51 @@
       <c r="N9" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O9" s="8">
+        <v>7</v>
+      </c>
+      <c r="P9" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q9" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S9" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>3</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="8">
         <v>70</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="8">
         <v>80</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="8">
         <v>4</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="8">
         <v>14</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="8">
         <v>0</v>
       </c>
       <c r="H10" s="7">
         <v>0</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>2</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>30</v>
       </c>
       <c r="K10" s="7">
@@ -2069,40 +2286,55 @@
       <c r="N10" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O10" s="8">
+        <v>7</v>
+      </c>
+      <c r="P10" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q10" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S10" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <f>15*0.43+3*0.01+5*0.56</f>
         <v>9.2800000000000011</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>70</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>80</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <f>0.43*4+0.01*7+0.56*20</f>
         <v>12.990000000000002</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <f>0.43*4.5+0.01*15.9+0.56*15.9</f>
         <v>10.998000000000001</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>0</v>
       </c>
       <c r="H11" s="7">
         <v>0</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <f>0.43*60+0.01*0+0.56*0</f>
         <v>25.8</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <f>I11*4</f>
         <v>103.2</v>
       </c>
@@ -2118,36 +2350,51 @@
       <c r="N11" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O11" s="8">
+        <v>7</v>
+      </c>
+      <c r="P11" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q11" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S11" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>10</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>120</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>280</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>2</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>9.9</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>0</v>
       </c>
       <c r="H12" s="7">
         <v>0</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>60</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>180</v>
       </c>
       <c r="K12" s="7">
@@ -2162,36 +2409,51 @@
       <c r="N12" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O12" s="8">
+        <v>7</v>
+      </c>
+      <c r="P12" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R12" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>10</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>70</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>80</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>2</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>11.3</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0</v>
       </c>
       <c r="H13" s="7">
         <v>0</v>
       </c>
-      <c r="I13" s="9">
+      <c r="I13" s="8">
         <v>120</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>360</v>
       </c>
       <c r="K13" s="7">
@@ -2206,36 +2468,51 @@
       <c r="N13" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O13" s="8">
+        <v>7</v>
+      </c>
+      <c r="P13" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q13" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S13" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="9">
-        <v>0</v>
-      </c>
-      <c r="C14" s="9">
+      <c r="B14" s="8">
+        <v>0</v>
+      </c>
+      <c r="C14" s="8">
         <v>70</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>0</v>
       </c>
       <c r="E14" s="8">
         <v>0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="8">
         <v>6.6</v>
       </c>
-      <c r="G14" s="9">
-        <v>0</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="8">
         <v>100</v>
       </c>
-      <c r="I14" s="9">
-        <v>0</v>
-      </c>
-      <c r="J14" s="9">
+      <c r="I14" s="8">
+        <v>0</v>
+      </c>
+      <c r="J14" s="8">
         <v>0</v>
       </c>
       <c r="K14" s="7">
@@ -2250,273 +2527,499 @@
       <c r="N14" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="O14" s="8">
+        <v>7</v>
+      </c>
+      <c r="P14" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q14" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S14" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" s="8">
+        <v>0</v>
+      </c>
+      <c r="C15" s="8">
+        <v>70</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0</v>
+      </c>
+      <c r="F15" s="8">
+        <v>6.6</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="8">
+        <v>100</v>
+      </c>
+      <c r="I15" s="8">
+        <v>0</v>
+      </c>
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>0</v>
+      </c>
+      <c r="L15" s="7">
+        <v>0</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
+        <v>7</v>
+      </c>
+      <c r="P15" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q15" s="9">
+        <v>0.222</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S15" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="8">
+        <v>0</v>
+      </c>
+      <c r="C16" s="8">
+        <v>70</v>
+      </c>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+      <c r="E16" s="8">
+        <v>0</v>
+      </c>
+      <c r="F16" s="8">
+        <v>6.6</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="8">
+        <v>100</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="8">
+        <v>7</v>
+      </c>
+      <c r="P16" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q16" s="9">
+        <v>0.106</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S16" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="9">
-        <v>0</v>
-      </c>
-      <c r="C15" s="9">
+      <c r="B17" s="8">
+        <v>0</v>
+      </c>
+      <c r="C17" s="8">
         <v>35</v>
       </c>
-      <c r="D15" s="9">
-        <v>0</v>
-      </c>
-      <c r="E15" s="9">
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
         <v>1</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F17" s="8">
         <v>2.9</v>
       </c>
-      <c r="G15" s="9">
-        <v>0</v>
-      </c>
-      <c r="H15" s="7">
-        <v>0</v>
-      </c>
-      <c r="I15" s="9">
-        <v>0</v>
-      </c>
-      <c r="J15" s="9">
-        <v>0</v>
-      </c>
-      <c r="K15" s="7">
-        <v>0</v>
-      </c>
-      <c r="L15" s="7">
-        <v>0</v>
-      </c>
-      <c r="M15" s="7">
-        <v>0</v>
-      </c>
-      <c r="N15" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="5" t="s">
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="7">
+        <v>0</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0</v>
+      </c>
+      <c r="J17" s="8">
+        <v>0</v>
+      </c>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
+      <c r="M17" s="7">
+        <v>0</v>
+      </c>
+      <c r="N17" s="7">
+        <v>0</v>
+      </c>
+      <c r="O17" s="8">
+        <v>7</v>
+      </c>
+      <c r="P17" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q17" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S17" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="9">
-        <v>0</v>
-      </c>
-      <c r="C16" s="9">
+      <c r="B18" s="8">
+        <v>0</v>
+      </c>
+      <c r="C18" s="8">
         <v>70</v>
       </c>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-      <c r="E16" s="9">
-        <v>0</v>
-      </c>
-      <c r="F16" s="9">
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0</v>
+      </c>
+      <c r="F18" s="8">
         <v>5.7</v>
       </c>
-      <c r="G16" s="9">
-        <v>0</v>
-      </c>
-      <c r="H16" s="7">
-        <v>0</v>
-      </c>
-      <c r="I16" s="9">
-        <v>0</v>
-      </c>
-      <c r="J16" s="9">
-        <v>0</v>
-      </c>
-      <c r="K16" s="7">
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="7">
+        <v>0</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0</v>
+      </c>
+      <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18" s="7">
         <v>100</v>
       </c>
-      <c r="L16" s="7">
-        <v>0</v>
-      </c>
-      <c r="M16" s="7">
-        <v>0</v>
-      </c>
-      <c r="N16" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+      <c r="L18" s="7">
+        <v>0</v>
+      </c>
+      <c r="M18" s="7">
+        <v>0</v>
+      </c>
+      <c r="N18" s="7">
+        <v>0</v>
+      </c>
+      <c r="O18" s="8">
+        <v>7</v>
+      </c>
+      <c r="P18" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q18" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S18" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B19" s="8">
         <v>15</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C19" s="8">
         <f>C11</f>
         <v>70</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D19" s="8">
         <f>D11</f>
         <v>80</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E19" s="8">
         <v>20</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F19" s="8">
         <v>16.2</v>
       </c>
-      <c r="G17" s="9">
+      <c r="G19" s="8">
         <f>G9</f>
         <v>16.5</v>
       </c>
-      <c r="H17" s="7">
-        <v>0</v>
-      </c>
-      <c r="I17" s="9">
+      <c r="H19" s="7">
+        <v>0</v>
+      </c>
+      <c r="I19" s="8">
         <v>3</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J19" s="8">
         <v>60</v>
       </c>
-      <c r="K17" s="7">
-        <v>0</v>
-      </c>
-      <c r="L17" s="7">
-        <v>0</v>
-      </c>
-      <c r="M17" s="7">
-        <v>0</v>
-      </c>
-      <c r="N17" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="5" t="s">
+      <c r="K19" s="7">
+        <v>0</v>
+      </c>
+      <c r="L19" s="7">
+        <v>0</v>
+      </c>
+      <c r="M19" s="7">
+        <v>0</v>
+      </c>
+      <c r="N19" s="7">
+        <v>0</v>
+      </c>
+      <c r="O19" s="8">
+        <v>7</v>
+      </c>
+      <c r="P19" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R19" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S19" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B20" s="8">
         <v>3</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C20" s="8">
         <v>70</v>
       </c>
-      <c r="D18" s="9">
+      <c r="D20" s="8">
         <v>80</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E20" s="8">
         <v>7</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F20" s="8">
         <v>10.8</v>
       </c>
-      <c r="G18" s="9">
-        <v>0</v>
-      </c>
-      <c r="H18" s="7">
-        <v>0</v>
-      </c>
-      <c r="I18" s="9">
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="7">
+        <v>0</v>
+      </c>
+      <c r="I20" s="8">
         <v>2</v>
       </c>
-      <c r="J18" s="9">
+      <c r="J20" s="8">
         <v>30</v>
       </c>
-      <c r="K18" s="7">
-        <v>0</v>
-      </c>
-      <c r="L18" s="7">
-        <v>0</v>
-      </c>
-      <c r="M18" s="7">
-        <v>0</v>
-      </c>
-      <c r="N18" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
+      <c r="K20" s="7">
+        <v>0</v>
+      </c>
+      <c r="L20" s="7">
+        <v>0</v>
+      </c>
+      <c r="M20" s="7">
+        <v>0</v>
+      </c>
+      <c r="N20" s="7">
+        <v>0</v>
+      </c>
+      <c r="O20" s="8">
+        <v>7</v>
+      </c>
+      <c r="P20" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q20" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R20" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S20" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B21" s="8">
         <v>5</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C21" s="8">
         <v>70</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D21" s="8">
         <v>80</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E21" s="8">
         <v>2</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F21" s="8">
         <v>6.9</v>
       </c>
-      <c r="G19" s="9">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7">
-        <v>0</v>
-      </c>
-      <c r="I19" s="9">
-        <v>0</v>
-      </c>
-      <c r="J19" s="9">
-        <v>0</v>
-      </c>
-      <c r="K19" s="7">
-        <v>0</v>
-      </c>
-      <c r="L19" s="7">
-        <v>0</v>
-      </c>
-      <c r="M19" s="7">
-        <v>0</v>
-      </c>
-      <c r="N19" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+      <c r="G21" s="8">
+        <v>0</v>
+      </c>
+      <c r="H21" s="7">
+        <v>0</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0</v>
+      </c>
+      <c r="J21" s="8">
+        <v>0</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="7">
+        <v>0</v>
+      </c>
+      <c r="M21" s="7">
+        <v>0</v>
+      </c>
+      <c r="N21" s="7">
+        <v>0</v>
+      </c>
+      <c r="O21" s="8">
+        <v>7</v>
+      </c>
+      <c r="P21" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q21" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R21" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S21" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B22" s="8">
         <v>10</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C22" s="8">
         <v>70</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D22" s="8">
         <v>80</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E22" s="8">
         <v>4</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F22" s="8">
         <v>12.5</v>
       </c>
-      <c r="G20" s="9">
-        <v>0</v>
-      </c>
-      <c r="H20" s="7">
-        <v>0</v>
-      </c>
-      <c r="I20" s="9">
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
         <v>2</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J22" s="8">
         <v>30</v>
       </c>
-      <c r="K20" s="7">
-        <v>0</v>
-      </c>
-      <c r="L20" s="7">
-        <v>0</v>
-      </c>
-      <c r="M20" s="7">
-        <v>0</v>
-      </c>
-      <c r="N20" s="7">
-        <v>0</v>
-      </c>
+      <c r="K22" s="7">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7">
+        <v>0</v>
+      </c>
+      <c r="M22" s="7">
+        <v>0</v>
+      </c>
+      <c r="N22" s="7">
+        <v>0</v>
+      </c>
+      <c r="O22" s="8">
+        <v>7</v>
+      </c>
+      <c r="P22" s="7">
+        <v>15</v>
+      </c>
+      <c r="Q22" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="R22" s="10">
+        <v>0.83</v>
+      </c>
+      <c r="S22" s="7">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q23" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2525,6 +3028,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C4119BA2A2C9A34A9ABDCD539C093B2A" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2036187cb88b360b5a6de576d0a5f2f7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="be70d004-d1e5-4317-a402-eff109a4a2bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e63961df46f11abd186e13992df6f3c7" ns3:_="">
     <xsd:import namespace="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
@@ -2694,22 +3212,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A02AC8DD-FE6B-486F-A4E4-4D415B112715}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2725,28 +3252,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FDE0E5F9-FF42-4597-A9B4-295F640F8C60}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50FB2592-98F2-47F2-9116-BDE7AE919D54}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="be70d004-d1e5-4317-a402-eff109a4a2bb"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>